<commit_message>
added completion of fixes on excel replication
</commit_message>
<xml_diff>
--- a/src/test/resources/complex/Complex_generated.xlsx
+++ b/src/test/resources/complex/Complex_generated.xlsx
@@ -13,9 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="76">
   <si>
     <t>Pension Asset Investment Results (Summary)</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Shareholder Name</t>
@@ -189,9 +192,6 @@
   </si>
   <si>
     <t>Record Date</t>
-  </si>
-  <si>
-    <t>09/03/2022</t>
   </si>
   <si>
     <t>Code</t>
@@ -252,7 +252,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0_ "/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="213">
     <font>
       <sz val="11.0"/>
@@ -2665,7 +2668,7 @@
     <xf numFmtId="0" fontId="178" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="179" fillId="4" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="165" fontId="179" fillId="4" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="180" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
@@ -2814,134 +2817,192 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="10"/>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="C3" s="11" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>1</v>
+      </c>
       <c r="G3" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>1</v>
+      </c>
       <c r="I3" s="17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="C4" s="18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="19" t="n">
         <v>1011.0</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="23"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>1</v>
+      </c>
       <c r="I4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="25"/>
+        <v>11</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="5">
       <c r="C5" s="26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="31"/>
+        <v>16</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>1</v>
+      </c>
       <c r="I5" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
+        <v>17</v>
+      </c>
+      <c r="J5" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6"/>
     <row r="7">
-      <c r="B7" s="35"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>1</v>
+      </c>
       <c r="D7" s="37" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="39"/>
+        <v>19</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>1</v>
+      </c>
       <c r="G7" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>1</v>
+      </c>
       <c r="I7" s="42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J7" s="43" t="s">
-        <v>21</v>
-      </c>
-      <c r="K7" s="44"/>
+        <v>22</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>1</v>
+      </c>
       <c r="L7" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="46"/>
+        <v>23</v>
+      </c>
+      <c r="N7" s="46" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
-      <c r="B8" s="47"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49"/>
+      <c r="B8" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>1</v>
+      </c>
       <c r="E8" s="50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="51" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G8" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="57"/>
+      <c r="I8" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="57" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" s="58" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="64" t="n">
         <v>1.5386579E7</v>
@@ -2967,14 +3028,16 @@
       <c r="L9" s="73">
         <f>J9/J16</f>
       </c>
-      <c r="O9" s="74"/>
+      <c r="O9" s="74" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" s="59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="64" t="n">
         <v>1.517092239E9</v>
@@ -3004,10 +3067,10 @@
     </row>
     <row r="11">
       <c r="B11" s="60" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="64" t="n">
         <v>1.46077741E8</v>
@@ -3037,10 +3100,10 @@
     </row>
     <row r="12">
       <c r="B12" s="61" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" s="64" t="n">
         <v>1.44401851E8</v>
@@ -3070,10 +3133,10 @@
     </row>
     <row r="13">
       <c r="B13" s="62" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="64" t="n">
         <v>1.332687412E9</v>
@@ -3102,37 +3165,81 @@
       <c r="O13" s="72"/>
     </row>
     <row r="14">
-      <c r="B14" s="75"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="82"/>
-      <c r="J14" s="83"/>
-      <c r="L14" s="84"/>
-      <c r="O14" s="85"/>
+      <c r="B14" s="75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="78" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="79" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="82" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="85" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
-      <c r="B15" s="86"/>
-      <c r="C15" s="87"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="94"/>
-      <c r="L15" s="95"/>
-      <c r="O15" s="96"/>
+      <c r="B15" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="96" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" s="97" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="98" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="99">
         <f>SUM(D9:D13)</f>
@@ -3160,33 +3267,47 @@
       </c>
     </row>
     <row r="17">
-      <c r="G17" s="107"/>
+      <c r="G17" s="107" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="18">
-      <c r="E18" s="108"/>
-      <c r="I18" s="109"/>
+      <c r="E18" s="108" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="109" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" s="110" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="111"/>
+        <v>39</v>
+      </c>
+      <c r="C20" s="111" t="s">
+        <v>1</v>
+      </c>
       <c r="I20" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="113"/>
+        <v>40</v>
+      </c>
+      <c r="J20" s="113" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" s="114" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="115"/>
+        <v>41</v>
+      </c>
+      <c r="C21" s="115" t="s">
+        <v>1</v>
+      </c>
       <c r="D21" s="116" t="n">
         <v>0.0</v>
       </c>
-      <c r="E21" s="117"/>
+      <c r="E21" s="117" t="s">
+        <v>1</v>
+      </c>
       <c r="I21" s="118" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="J21" s="119" t="n">
         <v>3.2560944E7</v>
@@ -3194,15 +3315,19 @@
     </row>
     <row r="22">
       <c r="B22" s="120" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="121"/>
+        <v>43</v>
+      </c>
+      <c r="C22" s="121" t="s">
+        <v>1</v>
+      </c>
       <c r="D22" s="122" t="n">
         <v>7833894.0</v>
       </c>
-      <c r="E22" s="123"/>
+      <c r="E22" s="123" t="s">
+        <v>1</v>
+      </c>
       <c r="I22" s="124" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J22" s="125" t="n">
         <v>4.0394838E7</v>
@@ -3210,14 +3335,16 @@
     </row>
     <row r="23">
       <c r="B23" s="126" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="127"/>
+        <v>45</v>
+      </c>
+      <c r="C23" s="127" t="s">
+        <v>1</v>
+      </c>
       <c r="D23" s="128" t="n">
         <v>0.0</v>
       </c>
       <c r="I23" s="129" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J23" s="130" t="n">
         <v>-7833894.0</v>
@@ -3225,99 +3352,163 @@
     </row>
     <row r="24">
       <c r="B24" s="131" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="132"/>
+        <v>47</v>
+      </c>
+      <c r="C24" s="132" t="s">
+        <v>1</v>
+      </c>
       <c r="D24" s="133" t="n">
         <v>-7833894.0</v>
       </c>
       <c r="I24" s="134" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J24" s="135" t="n">
         <v>0.0</v>
       </c>
-      <c r="K24" s="136"/>
+      <c r="K24" s="136" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" s="137" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="138"/>
-      <c r="D27" s="139"/>
-      <c r="E27" s="140"/>
-      <c r="F27" s="141"/>
+        <v>49</v>
+      </c>
+      <c r="C27" s="138" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="139" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="141" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="28">
-      <c r="B28" s="142"/>
-      <c r="C28" s="143"/>
+      <c r="B28" s="142" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="143" t="s">
+        <v>1</v>
+      </c>
       <c r="D28" s="144" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E28" s="145" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="146"/>
+        <v>51</v>
+      </c>
+      <c r="F28" s="146" t="s">
+        <v>1</v>
+      </c>
       <c r="G28" s="147" t="s">
-        <v>51</v>
-      </c>
-      <c r="H28" s="148"/>
+        <v>52</v>
+      </c>
+      <c r="H28" s="148" t="s">
+        <v>1</v>
+      </c>
       <c r="I28" s="149" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J28" s="150" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="151" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="152"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="156"/>
-      <c r="H29" s="157"/>
-      <c r="I29" s="158"/>
-      <c r="J29" s="159"/>
+        <v>55</v>
+      </c>
+      <c r="C29" s="152" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="153" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="154" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="155" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="157" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="159" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="30">
-      <c r="G30" s="160"/>
-      <c r="I30" s="161"/>
-      <c r="J30" s="162"/>
+      <c r="G30" s="160" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="161" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="162" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" s="163" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="164"/>
-      <c r="D31" s="165"/>
-      <c r="G31" s="166"/>
+        <v>56</v>
+      </c>
+      <c r="C31" s="164" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="165" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="166" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="32">
-      <c r="G32" s="167"/>
+      <c r="G32" s="167" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
-      <c r="G33" s="168"/>
+      <c r="G33" s="168" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
-      <c r="G34" s="169"/>
+      <c r="G34" s="169" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="35">
-      <c r="G35" s="170"/>
+      <c r="G35" s="170" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="36">
-      <c r="G36" s="171"/>
+      <c r="G36" s="171" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="37">
-      <c r="G37" s="172"/>
+      <c r="G37" s="172" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="38">
-      <c r="G38" s="173"/>
+      <c r="G38" s="173" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
-      <c r="G39" s="174"/>
+      <c r="G39" s="174" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3372,34 +3563,42 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="175"/>
+      <c r="A1" s="175" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="176" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="177" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="178"/>
+        <v>4</v>
+      </c>
+      <c r="C2" s="178" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="179" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="180" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="181"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="181" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="182" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="183" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="184"/>
+      <c r="B4" s="183" t="n">
+        <v>44628.666666666664</v>
+      </c>
+      <c r="C4" s="184" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="185" t="s">
@@ -3428,8 +3627,12 @@
       <c r="B7" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="201"/>
-      <c r="D7" s="202"/>
+      <c r="C7" s="201" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="202" t="s">
+        <v>1</v>
+      </c>
       <c r="E7" s="199" t="n">
         <v>1.31622258E8</v>
       </c>
@@ -3502,34 +3705,70 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="203"/>
-      <c r="C12" s="204"/>
-      <c r="D12" s="205"/>
-      <c r="E12" s="206"/>
+      <c r="A12" s="203" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="204" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="205" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="206" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="207"/>
-      <c r="C13" s="208"/>
-      <c r="D13" s="209"/>
-      <c r="E13" s="210"/>
+      <c r="A13" s="207" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="208" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="209" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="210" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
-      <c r="C14" s="211"/>
-      <c r="D14" s="212"/>
-      <c r="E14" s="213"/>
+      <c r="C14" s="211" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="212" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="213" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="214"/>
-      <c r="C15" s="215"/>
-      <c r="D15" s="216"/>
-      <c r="E15" s="217"/>
+      <c r="A15" s="214" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="216" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="217" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
-      <c r="C16" s="218"/>
-      <c r="D16" s="219"/>
+      <c r="C16" s="218" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="219" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
-      <c r="E21" s="220"/>
+      <c r="E21" s="220" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="false"/>

</xml_diff>

<commit_message>
Refactoring clean code on writers and formatters
</commit_message>
<xml_diff>
--- a/src/test/resources/complex/Complex_generated.xlsx
+++ b/src/test/resources/complex/Complex_generated.xlsx
@@ -256,7 +256,7 @@
     <numFmt numFmtId="164" formatCode="0_ "/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="213">
+  <fonts count="219">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -817,6 +817,16 @@
     <font>
       <name val="MS P明朝"/>
       <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
       <color indexed="17"/>
     </font>
     <font>
@@ -1063,6 +1073,26 @@
       <name val="ＭＳ Ｐゴシック"/>
       <sz val="10.0"/>
       <color indexed="0"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="MS P明朝"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
     </font>
     <font>
       <name val="MS P明朝"/>
@@ -1456,7 +1486,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="68">
+  <borders count="173">
     <border>
       <left/>
       <right/>
@@ -1465,648 +1495,1632 @@
       <diagonal/>
     </border>
     <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
       <top>
         <color indexed="8"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
       <top>
         <color indexed="8"/>
       </top>
       <bottom>
         <color indexed="8"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom>
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right>
         <color indexed="8"/>
       </right>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top>
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom>
         <color indexed="8"/>
       </bottom>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right>
         <color indexed="8"/>
       </right>
-    </border>
-    <border>
-      <top>
-        <color indexed="8"/>
-      </top>
-      <bottom>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
     </border>
     <border>
-      <bottom>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
     </border>
     <border>
+      <right style="thin"/>
+      <top style="medium"/>
+    </border>
+    <border>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right>
         <color indexed="8"/>
       </right>
-      <bottom>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
     </border>
     <border>
+      <right style="medium"/>
+      <top style="thin"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right>
         <color indexed="8"/>
       </right>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
     </border>
     <border>
-      <top>
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
     </border>
     <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top>
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <left style="medium"/>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="8"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom>
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <right>
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="medium"/>
-      <right>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -2120,39 +3134,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="9" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
@@ -2164,622 +3178,640 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="9" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="24" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="24" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="bottom"/>
     </xf>
-    <xf numFmtId="38" fontId="25" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="25" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="49" fontId="28" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="32" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="32" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="bottom"/>
     </xf>
-    <xf numFmtId="38" fontId="33" fillId="10" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="33" fillId="10" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="7" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="34" fillId="7" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="21" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="20" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="23" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="25" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="37" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="37" fillId="7" borderId="31" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="40" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="41" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="42" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="42" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="43" fillId="7" borderId="29" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="43" fillId="7" borderId="44" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="44" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="7" borderId="30" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="44" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="7" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="7" borderId="35" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="46" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="7" borderId="55" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="7" borderId="36" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="48" fillId="7" borderId="61" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="49" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="49" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="50" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="50" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="51" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="52" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="52" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="53" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="54" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="54" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="55" fillId="7" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="55" fillId="7" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="56" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="7" borderId="44" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="56" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="7" borderId="88" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="58" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="58" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="58" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="58" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="58" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="7" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="59" fillId="7" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="true" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="60" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="60" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="61" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="61" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="62" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="62" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="63" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="63" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="64" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="64" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="65" fillId="10" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="65" fillId="10" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="66" fillId="10" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="66" fillId="10" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="67" fillId="10" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="10" fontId="67" fillId="10" borderId="94" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="68" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="69" fillId="10" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="3" fontId="68" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="69" fillId="10" borderId="94" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="70" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="71" fillId="7" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="3" fontId="70" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="7" borderId="98" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="72" fillId="7" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="72" fillId="7" borderId="102" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="true" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="73" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="73" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="74" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="74" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="75" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="75" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="76" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="76" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="77" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="77" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="78" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="78" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="79" fillId="10" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="79" fillId="10" borderId="102" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="80" fillId="10" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="10" fontId="80" fillId="10" borderId="110" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="81" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="82" fillId="7" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="3" fontId="81" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="82" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="7" borderId="98" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="83" fillId="7" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="84" fillId="7" borderId="102" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="true" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="84" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="85" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="85" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="86" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="86" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="87" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="87" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="88" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="88" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="89" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="89" fillId="10" borderId="49" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="90" fillId="10" borderId="106" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="90" fillId="10" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="91" fillId="10" borderId="102" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="91" fillId="10" borderId="51" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="10" fontId="92" fillId="10" borderId="110" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="92" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="7" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="3" fontId="93" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="7" borderId="115" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="94" fillId="7" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="96" fillId="7" borderId="120" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="95" fillId="13" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="97" fillId="13" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="96" fillId="16" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="98" fillId="16" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="97" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="99" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="98" fillId="16" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="100" fillId="16" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="99" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="164" fontId="101" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="100" fillId="13" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="102" fillId="13" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="101" fillId="13" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="103" fillId="13" borderId="120" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="102" fillId="19" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="10" fontId="104" fillId="19" borderId="130" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="103" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="104" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="105" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="110" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="105" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="106" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="107" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="7" borderId="31" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="111" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="113" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="112" fillId="10" borderId="29" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="114" fillId="10" borderId="44" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="113" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="114" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="115" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="7" borderId="31" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="115" fillId="16" borderId="29" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="117" fillId="16" borderId="44" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="116" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="118" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="117" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="119" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="118" fillId="10" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="120" fillId="10" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="119" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="120" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="121" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="121" fillId="16" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="123" fillId="16" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="122" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="124" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="123" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="125" fillId="7" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="124" fillId="10" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="126" fillId="10" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="125" fillId="7" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="127" fillId="7" borderId="69" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="126" fillId="16" borderId="43" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="128" fillId="16" borderId="82" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="127" fillId="7" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="129" fillId="7" borderId="115" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="128" fillId="7" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="130" fillId="7" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="129" fillId="19" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="131" fillId="19" borderId="120" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="130" fillId="7" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="132" fillId="7" borderId="115" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="131" fillId="16" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="133" fillId="16" borderId="120" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="132" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="133" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="134" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="135" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="136" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="137" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="138" fillId="7" borderId="56" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="134" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="140" fillId="7" borderId="135" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="139" fillId="7" borderId="57" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="141" fillId="7" borderId="140" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="140" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="142" fillId="7" borderId="31" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="141" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="143" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="142" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="144" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="143" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="145" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="144" fillId="7" borderId="59" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="146" fillId="7" borderId="146" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="145" fillId="7" borderId="27" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="147" fillId="7" borderId="38" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="146" fillId="7" borderId="29" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="148" fillId="7" borderId="44" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="147" fillId="7" borderId="62" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="149" fillId="7" borderId="151" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="148" fillId="7" borderId="64" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="150" fillId="7" borderId="157" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="149" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="151" fillId="10" borderId="115" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="150" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="152" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="151" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="153" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="152" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="154" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="153" fillId="10" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="155" fillId="10" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="154" fillId="13" borderId="52" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="156" fillId="13" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="155" fillId="13" borderId="53" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="157" fillId="13" borderId="120" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="156" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="157" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="158" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="159" fillId="7" borderId="65" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="158" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="160" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="7" borderId="162" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="160" fillId="7" borderId="66" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="162" fillId="7" borderId="167" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="161" fillId="10" borderId="67" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="163" fillId="10" borderId="172" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="162" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="163" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="164" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="165" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="166" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="167" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="168" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="164" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="166" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="168" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="170" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="169" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="170" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="171" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="172" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="173" fillId="7" borderId="9" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="171" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="172" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="173" fillId="10" borderId="94" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="174" fillId="16" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="175" fillId="16" borderId="125" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="right" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="176" fillId="19" borderId="130" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="right" wrapText="true" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="177" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="179" fillId="7" borderId="9" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="174" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="175" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="176" fillId="4" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="177" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="178" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="179" fillId="4" borderId="14" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="180" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="181" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="4" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="183" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="185" fillId="4" borderId="15" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="left" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="180" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="181" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="186" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="187" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="182" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="188" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="183" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="189" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="184" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="190" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="185" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="38" fontId="191" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="186" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="192" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="center" wrapText="false" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="187" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="193" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="188" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="194" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="189" fillId="22" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="190" fillId="22" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="191" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="195" fillId="22" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="196" fillId="22" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="197" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="192" fillId="4" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="198" fillId="4" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="193" fillId="22" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="194" fillId="22" borderId="41" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="195" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="199" fillId="22" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="200" fillId="22" borderId="76" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="201" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="196" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="197" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="198" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="199" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="202" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="203" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="204" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="205" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="true" vertical="center"/>
     </xf>
-    <xf numFmtId="40" fontId="200" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="201" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="202" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="203" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="204" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="205" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="206" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="207" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="208" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="209" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="210" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="211" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
-      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
-    </xf>
-    <xf numFmtId="38" fontId="212" fillId="4" borderId="5" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="40" fontId="206" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="207" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="208" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="209" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="210" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="211" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="212" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="213" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="214" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="215" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="216" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="217" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="218" fillId="4" borderId="4" xfId="0" applyFont="true" applyFill="true" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
       <alignment shrinkToFit="false" horizontal="general" wrapText="false" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3025,7 +4057,7 @@
       <c r="J9" s="70" t="n">
         <v>8060568.0</v>
       </c>
-      <c r="L9" s="73">
+      <c r="L9" s="177">
         <f>J9/J16</f>
       </c>
       <c r="O9" s="74" t="s">
@@ -3164,7 +4196,7 @@
       </c>
       <c r="O13" s="72"/>
     </row>
-    <row r="14">
+    <row r="14" s="86" customFormat="true">
       <c r="B14" s="75" t="s">
         <v>1</v>
       </c>
@@ -3199,314 +4231,314 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="86" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="87" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="90" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="91" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="92" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="L15" s="95" t="s">
-        <v>1</v>
-      </c>
-      <c r="O15" s="96" t="s">
+    <row r="15" s="98" customFormat="true">
+      <c r="B15" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="88" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="92" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="95" t="s">
+        <v>1</v>
+      </c>
+      <c r="L15" s="96" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" s="97" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="99" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="99">
+      <c r="D16" s="101">
         <f>SUM(D9:D13)</f>
       </c>
-      <c r="E16" s="100">
+      <c r="E16" s="178">
         <f>D21</f>
       </c>
-      <c r="F16" s="101" t="n">
+      <c r="F16" s="103" t="n">
         <v>0.0</v>
       </c>
-      <c r="G16" s="102">
+      <c r="G16" s="179">
         <f>D21+D22</f>
       </c>
-      <c r="H16" s="103" t="n">
+      <c r="H16" s="105" t="n">
         <v>1.0</v>
       </c>
-      <c r="I16" s="104">
+      <c r="I16" s="106">
         <f>SUM(I9:I13)</f>
       </c>
-      <c r="J16" s="105">
+      <c r="J16" s="107">
         <f>SUM(J9:J13)</f>
       </c>
-      <c r="L16" s="106">
+      <c r="L16" s="180">
         <f>SUM(L9:L13)</f>
       </c>
     </row>
     <row r="17">
-      <c r="G17" s="107" t="s">
+      <c r="G17" s="109" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18">
-      <c r="E18" s="108" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="109" t="s">
+      <c r="E18" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="111" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="110" t="s">
+      <c r="B20" s="112" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="111" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" s="112" t="s">
+      <c r="C20" s="113" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="113" t="s">
+      <c r="J20" s="115" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="114" t="s">
+      <c r="B21" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="115" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="116" t="n">
+      <c r="C21" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="118" t="n">
         <v>0.0</v>
       </c>
-      <c r="E21" s="117" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="118" t="s">
+      <c r="E21" s="119" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="J21" s="119" t="n">
+      <c r="J21" s="121" t="n">
         <v>3.2560944E7</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="120" t="s">
+      <c r="B22" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="121" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="122" t="n">
+      <c r="C22" s="123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="124" t="n">
         <v>7833894.0</v>
       </c>
-      <c r="E22" s="123" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="124" t="s">
+      <c r="E22" s="125" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="126" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="125" t="n">
+      <c r="J22" s="127" t="n">
         <v>4.0394838E7</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="126" t="s">
+      <c r="B23" s="128" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="127" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="128" t="n">
+      <c r="C23" s="129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="130" t="n">
         <v>0.0</v>
       </c>
-      <c r="I23" s="129" t="s">
+      <c r="I23" s="131" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="130" t="n">
+      <c r="J23" s="132" t="n">
         <v>-7833894.0</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="131" t="s">
+      <c r="B24" s="133" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="132" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="133" t="n">
+      <c r="C24" s="134" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="135" t="n">
         <v>-7833894.0</v>
       </c>
-      <c r="I24" s="134" t="s">
+      <c r="I24" s="136" t="s">
         <v>48</v>
       </c>
-      <c r="J24" s="135" t="n">
+      <c r="J24" s="137" t="n">
         <v>0.0</v>
       </c>
-      <c r="K24" s="136" t="s">
+      <c r="K24" s="138" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="27">
-      <c r="B27" s="137" t="s">
+      <c r="B27" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="138" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="139" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27" s="140" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="141" t="s">
+      <c r="C27" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="141" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="142" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="143" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="142" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="143" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="144" t="s">
+      <c r="B28" s="144" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="145" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="146" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="145" t="s">
+      <c r="E28" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="146" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="147" t="s">
+      <c r="F28" s="148" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="149" t="s">
         <v>52</v>
       </c>
-      <c r="H28" s="148" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" s="149" t="s">
+      <c r="H28" s="150" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="J28" s="150" t="s">
+      <c r="J28" s="152" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29">
-      <c r="B29" s="151" t="s">
+      <c r="B29" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="152" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="153" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="154" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="155" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="156" t="s">
-        <v>1</v>
-      </c>
-      <c r="H29" s="157" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="158" t="s">
-        <v>1</v>
-      </c>
-      <c r="J29" s="159" t="s">
+      <c r="C29" s="154" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="155" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="156" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="157" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="158" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="159" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" s="160" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" s="161" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="30">
-      <c r="G30" s="160" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" s="161" t="s">
-        <v>1</v>
-      </c>
-      <c r="J30" s="162" t="s">
+      <c r="G30" s="162" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="163" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="164" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="163" t="s">
+      <c r="B31" s="165" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="164" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="165" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="166" t="s">
+      <c r="C31" s="166" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="167" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="168" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="32">
-      <c r="G32" s="167" t="s">
+      <c r="G32" s="169" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="33">
-      <c r="G33" s="168" t="s">
+      <c r="G33" s="170" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="34">
-      <c r="G34" s="169" t="s">
+      <c r="G34" s="171" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="35">
-      <c r="G35" s="170" t="s">
+      <c r="G35" s="172" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="36">
-      <c r="G36" s="171" t="s">
+      <c r="G36" s="173" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="37">
-      <c r="G37" s="172" t="s">
+      <c r="G37" s="174" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="38">
-      <c r="G38" s="173" t="s">
+      <c r="G38" s="175" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="39">
-      <c r="G39" s="174" t="s">
+      <c r="G39" s="176" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3563,210 +4595,210 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="181" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="176" t="s">
+      <c r="A2" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="177" t="s">
+      <c r="B2" s="183" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="184" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="179" t="s">
+      <c r="A3" s="185" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="186" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="181" t="s">
+      <c r="C3" s="187" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="182" t="s">
+      <c r="A4" s="188" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="183" t="n">
+      <c r="B4" s="189" t="n">
         <v>44628.666666666664</v>
       </c>
-      <c r="C4" s="184" t="s">
+      <c r="C4" s="190" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="185" t="s">
+      <c r="A6" s="191" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="192" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="187" t="s">
+      <c r="C6" s="193" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="188" t="s">
+      <c r="D6" s="194" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="189" t="s">
+      <c r="E6" s="195" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="190" t="s">
+      <c r="F6" s="196" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="191" t="s">
+      <c r="A7" s="197" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="196" t="s">
+      <c r="B7" s="202" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="201" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="202" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="199" t="n">
+      <c r="C7" s="207" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="208" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="205" t="n">
         <v>1.31622258E8</v>
       </c>
-      <c r="F7" s="200" t="s">
+      <c r="F7" s="206" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="192" t="s">
+      <c r="A8" s="198" t="s">
         <v>65</v>
       </c>
-      <c r="B8" s="196" t="s">
+      <c r="B8" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="C8" s="197"/>
-      <c r="D8" s="198"/>
-      <c r="E8" s="199" t="n">
+      <c r="C8" s="203"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="205" t="n">
         <v>1.344762582E9</v>
       </c>
-      <c r="F8" s="200" t="s">
+      <c r="F8" s="206" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="196" t="s">
+      <c r="B9" s="202" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="197"/>
-      <c r="D9" s="198"/>
-      <c r="E9" s="199" t="n">
+      <c r="C9" s="203"/>
+      <c r="D9" s="204"/>
+      <c r="E9" s="205" t="n">
         <v>1.561662185E9</v>
       </c>
-      <c r="F9" s="200" t="s">
+      <c r="F9" s="206" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="194" t="s">
+      <c r="A10" s="200" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="196" t="s">
+      <c r="B10" s="202" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="197"/>
-      <c r="D10" s="198"/>
-      <c r="E10" s="199" t="n">
+      <c r="C10" s="203"/>
+      <c r="D10" s="204"/>
+      <c r="E10" s="205" t="n">
         <v>5.5714753E7</v>
       </c>
-      <c r="F10" s="200" t="s">
+      <c r="F10" s="206" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="195" t="s">
+      <c r="A11" s="201" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="202" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="197"/>
-      <c r="D11" s="198"/>
-      <c r="E11" s="199" t="n">
+      <c r="C11" s="203"/>
+      <c r="D11" s="204"/>
+      <c r="E11" s="205" t="n">
         <v>9.312652E7</v>
       </c>
-      <c r="F11" s="200" t="s">
+      <c r="F11" s="206" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="203" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="204" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="205" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" s="206" t="s">
+      <c r="A12" s="209" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="210" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="211" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="212" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="207" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="208" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="209" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" s="210" t="s">
+      <c r="A13" s="213" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="214" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="215" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="216" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14">
-      <c r="C14" s="211" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="212" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="213" t="s">
+      <c r="C14" s="217" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="218" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="219" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="214" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="215" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="216" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="217" t="s">
+      <c r="A15" s="220" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="221" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="222" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="223" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="16">
-      <c r="C16" s="218" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="219" t="s">
+      <c r="C16" s="224" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="225" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="21">
-      <c r="E21" s="220" t="s">
+      <c r="E21" s="226" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>